<commit_message>
Edited the project plan 4/6
</commit_message>
<xml_diff>
--- a/misc_files/CPSC224SpaceRaceProjectPlan.xlsx
+++ b/misc_files/CPSC224SpaceRaceProjectPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CourseProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPSC224_01_Group6\misc_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BDB5B-AA77-4211-B1C2-20A74C70C6FD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B208E8-4F14-4FE3-A471-E337E2246597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Edit project plan</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Work on resource icons</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -719,10 +725,14 @@
         <v>43196</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43194</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -738,17 +748,21 @@
         <v>43196</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43195</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>1.5</v>
@@ -757,9 +771,11 @@
         <v>43196</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43196</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,18 +792,32 @@
         <v>43196</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43196</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43203</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -882,6 +912,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1072,6 +1103,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC2685C84B160940930467983553E2DA" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64476ae877ed79da2175079bb3e4829a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0d329a-e114-4ba8-bee9-62c1c786fd9a" xmlns:ns3="013b2221-5078-4f34-9921-a0ecb049492d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="564df3335efcf36b4d09ae51e046af81" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
@@ -1252,43 +1319,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1305,29 +1361,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the schedule for 4/8 and added the project definition from blackboard
</commit_message>
<xml_diff>
--- a/misc_files/CPSC224SpaceRaceProjectPlan.xlsx
+++ b/misc_files/CPSC224SpaceRaceProjectPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPSC224_01_Group6\misc_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B208E8-4F14-4FE3-A471-E337E2246597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46AB839-9EE0-449A-A821-B9F82E5DE7F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WeekMar25" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -90,6 +90,42 @@
   </si>
   <si>
     <t>Work on resource icons</t>
+  </si>
+  <si>
+    <t>Work on test plan</t>
+  </si>
+  <si>
+    <t>Update buisness model to include expanations and test cases</t>
+  </si>
+  <si>
+    <t>Create design alternatives</t>
+  </si>
+  <si>
+    <t>Create design alternitive document</t>
+  </si>
+  <si>
+    <t>Create PlayGame.java</t>
+  </si>
+  <si>
+    <t>Create Hand.java</t>
+  </si>
+  <si>
+    <t>Create BuildPhase.java</t>
+  </si>
+  <si>
+    <t>Create SpacePhase.java</t>
+  </si>
+  <si>
+    <t>Create Scorecard.java</t>
+  </si>
+  <si>
+    <t>Create source code based off current UML spec</t>
+  </si>
+  <si>
+    <t>Create a design alternitive analysis document</t>
+  </si>
+  <si>
+    <t>Create a test plan document</t>
   </si>
 </sst>
 </file>
@@ -146,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -156,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3666E7-7A8F-4E6C-A921-3B9FDC8B896E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -920,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E23D512-EF74-419A-80CC-6C1FE1BF1CBE}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,109 +991,178 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43203</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43203</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43203</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43203</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43221</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43221</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43221</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43221</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43221</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1103,15 +1209,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
@@ -1136,6 +1233,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1320,14 +1426,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1340,6 +1438,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>